<commit_message>
commit upto 6 nov
</commit_message>
<xml_diff>
--- a/ajio_submission/page_home/utilities/test_data_fk.xlsx
+++ b/ajio_submission/page_home/utilities/test_data_fk.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Item_name</t>
   </si>
@@ -84,13 +84,79 @@
     <t>sunglass_men_menu</t>
   </si>
   <si>
-    <t>(By.LINK_TEXT, "/s/mhp-sunglasses-and-frames-4119-33682")</t>
-  </si>
-  <si>
     <t>sunglass_item</t>
   </si>
   <si>
     <t>(By.XPATH, "//div[text()='UV-Protected Full-Rim Computer Glasses']")</t>
+  </si>
+  <si>
+    <t>add_to_bag_sun_glass_item</t>
+  </si>
+  <si>
+    <t>cart_added_pop_up</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//div[@class='minicart-prod-name']")</t>
+  </si>
+  <si>
+    <t>ajio_logo_home</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//img[@alt='Ajio logo']")</t>
+  </si>
+  <si>
+    <t>cart_button_home_page</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//span[text()='ADD TO BAG']")</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//a/div[@class='ic-cart ']")</t>
+  </si>
+  <si>
+    <t>(By.LINK_TEXT, "Sunglasses &amp; Frames")</t>
+  </si>
+  <si>
+    <t>sun_glass_item_head</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//h1[@class='prod-name']")</t>
+  </si>
+  <si>
+    <t>sun_glass_item_price</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//div[@class='prod-sp']")</t>
+  </si>
+  <si>
+    <t>proceed_to_bag_btn</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//div[@aria-label='PROCEED TO BAG']")</t>
+  </si>
+  <si>
+    <t>cart_quantity_fetch</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "(//div[@class='minicart-value'])[3]")</t>
+  </si>
+  <si>
+    <t>cart_price_fetch</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//div[@class='minicart-totalamt']/span")</t>
+  </si>
+  <si>
+    <t>delete_btn_ship_page</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//a/span[text()='ROYAL SON']/../../../..//div[@class='product-delete']/div[contains(text(), 'Delete')]")</t>
+  </si>
+  <si>
+    <t>item_price_shipping_page</t>
+  </si>
+  <si>
+    <t>(By.XPATH, "//a/span[text()='ROYAL SON']/../../../..//div[@class='priceinfo']/div[2]")</t>
   </si>
 </sst>
 </file>
@@ -137,12 +203,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,16 +569,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="37.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="69" style="5" customWidth="1"/>
+    <col min="2" max="2" width="79.36328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -591,15 +665,103 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5">
       <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="5" customFormat="1" ht="15.5">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.5">
+      <c r="A14" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.5">
+      <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.5">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="5" customFormat="1" ht="15.5">
+      <c r="A18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="5" customFormat="1" ht="15.5">
+      <c r="A19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.5">
+      <c r="A21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.5">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>